<commit_message>
adding moorea sample info to the metadata
</commit_message>
<xml_diff>
--- a/Sample-Metadata.xlsx
+++ b/Sample-Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/Flow-Cytometer-Cell-Density-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C42E38-52EB-644A-ABDC-D7B254E5BCF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B869C9-37C7-4C44-A23C-746DE07872A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6620" yWindow="1680" windowWidth="28040" windowHeight="17440" xr2:uid="{AF6A4F39-E689-0544-9682-C4BD9A2C3630}"/>
+    <workbookView xWindow="5560" yWindow="1680" windowWidth="28040" windowHeight="17440" xr2:uid="{AF6A4F39-E689-0544-9682-C4BD9A2C3630}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="23">
   <si>
     <t>Sample ID</t>
   </si>
@@ -82,6 +82,27 @@
   </si>
   <si>
     <t>FlowCy Count?</t>
+  </si>
+  <si>
+    <t>Acropora spp.</t>
+  </si>
+  <si>
+    <t>~500 uL</t>
+  </si>
+  <si>
+    <t>E5 - Mo'orea</t>
+  </si>
+  <si>
+    <t>Do not use on FlowCy</t>
+  </si>
+  <si>
+    <t>Pocillopora spp.</t>
+  </si>
+  <si>
+    <t>Not diluted; Use minimal amount</t>
+  </si>
+  <si>
+    <t>Porites spp.</t>
   </si>
 </sst>
 </file>
@@ -440,19 +461,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D22A11-4E31-8D45-9D27-D1E89777C859}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.83203125" customWidth="1"/>
     <col min="6" max="6" width="22.1640625" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -567,18 +589,317 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>213</v>
+      </c>
       <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>173</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>139</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>178</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>190</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>377</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>257</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>259</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>205</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>262</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>242</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>340</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>216</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>80</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>